<commit_message>
Update for daily work
</commit_message>
<xml_diff>
--- a/Documents/config.xlsx
+++ b/Documents/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jsavory\Documents\GitHub\EA-FCRM-Utilities\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\EA-FCRM-Utilities\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA1D184-11DB-420F-9FC1-4E7255AEABAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9945" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,20 +268,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="Value" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B16" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B16" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="1"/>
-    <tableColumn id="2" name="Value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -582,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,10 +743,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +886,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -958,20 +959,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100040CE0A563279642A4E4F2E84657AA5A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="966060d0038f22014d5f48f1d075f2b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="97f96670-c786-4b18-bf2a-32c7cc01b520" xmlns:ns4="a1cc53fe-b63d-4766-a5c8-95c307055b81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="941117f54ba4546450a8d66256a0d267" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1274,6 +1261,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
   <ds:schemaRefs>
@@ -1294,22 +1295,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0C1FC-292C-435A-97DB-4855EBBBAAB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1328,4 +1313,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final commit for JS sprint 2
</commit_message>
<xml_diff>
--- a/Documents/config.xlsx
+++ b/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\EA-FCRM-Utilities\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA1D184-11DB-420F-9FC1-4E7255AEABAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74F7EB-9FF7-4034-A047-71B7CB8B7EA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="375" windowWidth="38715" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -107,13 +107,25 @@
   </si>
   <si>
     <t>Default end date days</t>
+  </si>
+  <si>
+    <t>BT URL</t>
+  </si>
+  <si>
+    <t>LSBUD URL</t>
+  </si>
+  <si>
+    <t>https://www.swns.bt.com/pls/mbe/welcome.home</t>
+  </si>
+  <si>
+    <t>https://onecall.linesearchbeforeudig.co.uk/uk-b4-en/Account/Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +151,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,7 +286,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
@@ -278,7 +296,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B16" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value" dataDxfId="0"/>
@@ -584,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,73 +681,89 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -744,10 +778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -828,65 +862,82 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="9">
-        <v>90</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B18" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -959,6 +1010,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100040CE0A563279642A4E4F2E84657AA5A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="966060d0038f22014d5f48f1d075f2b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="97f96670-c786-4b18-bf2a-32c7cc01b520" xmlns:ns4="a1cc53fe-b63d-4766-a5c8-95c307055b81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="941117f54ba4546450a8d66256a0d267" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1261,20 +1326,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
   <ds:schemaRefs>
@@ -1295,6 +1346,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0C1FC-292C-435A-97DB-4855EBBBAAB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1313,20 +1380,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
end of sprint 2 commit
</commit_message>
<xml_diff>
--- a/Documents/config.xlsx
+++ b/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\EA-FCRM-Utilities\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74F7EB-9FF7-4034-A047-71B7CB8B7EA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC3B6CA-E75A-4C1E-AD26-AE5ABFCB92B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="375" windowWidth="38715" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>https://onecall.linesearchbeforeudig.co.uk/uk-b4-en/Account/Login</t>
+  </si>
+  <si>
+    <t>Search Report Path</t>
+  </si>
+  <si>
+    <t>C:\temp\Search Report.xlsx</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
@@ -296,7 +302,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B19" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value" dataDxfId="0"/>
@@ -602,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="A9:B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,9 +767,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -778,10 +792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F15:F16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,9 +942,17 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1010,20 +1032,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100040CE0A563279642A4E4F2E84657AA5A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="966060d0038f22014d5f48f1d075f2b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="97f96670-c786-4b18-bf2a-32c7cc01b520" xmlns:ns4="a1cc53fe-b63d-4766-a5c8-95c307055b81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="941117f54ba4546450a8d66256a0d267" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1326,6 +1334,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
   <ds:schemaRefs>
@@ -1346,22 +1368,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0C1FC-292C-435A-97DB-4855EBBBAAB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1380,4 +1386,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit for end of day
</commit_message>
<xml_diff>
--- a/Documents/config.xlsx
+++ b/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\EA-FCRM-Utilities\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC3B6CA-E75A-4C1E-AD26-AE5ABFCB92B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE735022-EC5F-4FDE-A65A-D10813E8E7BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>C:\temp\Search Report.xlsx</t>
+  </si>
+  <si>
+    <t>Returns Queue</t>
   </si>
 </sst>
 </file>
@@ -292,7 +295,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,97 +690,105 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -794,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +981,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -1031,7 +1051,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Defra document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100040CE0A563279642A4E4F2E84657AA5A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="966060d0038f22014d5f48f1d075f2b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="662745e8-e224-48e8-a2e3-254862b8c2f5" xmlns:ns3="97f96670-c786-4b18-bf2a-32c7cc01b520" xmlns:ns4="a1cc53fe-b63d-4766-a5c8-95c307055b81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="941117f54ba4546450a8d66256a0d267" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1334,21 +1354,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a1cc53fe-b63d-4766-a5c8-95c307055b81"/>
@@ -1367,7 +1386,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0C1FC-292C-435A-97DB-4855EBBBAAB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1388,18 +1407,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFFE261-B0AE-4C8C-BD33-2EE90BE3D489}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push to save #2 work so far
</commit_message>
<xml_diff>
--- a/Documents/config.xlsx
+++ b/Documents/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\EA-FCRM-Utilities\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/jason_savory_defra_gov_uk/Documents/Jason - In Progress Work/EA-FCRM-Utilities/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE735022-EC5F-4FDE-A65A-D10813E8E7BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{AE735022-EC5F-4FDE-A65A-D10813E8E7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45EEAD96-D336-499F-9406-49D6BA173BD6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Returns Queue</t>
+  </si>
+  <si>
+    <t>DIGDAT URL</t>
+  </si>
+  <si>
+    <t>DIGDAT access expiry</t>
+  </si>
+  <si>
+    <t>Attachment Path</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
@@ -611,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,81 +723,97 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -990,65 +1015,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
-        </TermInfo>
-      </Terms>
-    </cf401361b24e474cb011be6eb76c0e76>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k85d23755b3a46b5a51451cf336b2e9b>
-    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Work Packages</Topic>
-    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
-    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
-        </TermInfo>
-      </Terms>
-    </ddeb1fd0a9ad4436a96525d34737dc44>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
-        </TermInfo>
-      </Terms>
-    </lae2bfa7b6474897ab4a53f76ea236c7>
-    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Value>10</Value>
-      <Value>9</Value>
-      <Value>8</Value>
-      <Value>7</Value>
-      <Value>6</Value>
-    </TaxCatchAll>
-    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DDTS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4b496496-8422-4e09-ae59-802e7f67f771</TermId>
-        </TermInfo>
-      </Terms>
-    </fe59e9859d6a491389c5b03567f5dda5>
-    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Digital Robotic Automation</Team>
-    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Community</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">144ac7d7-0b9a-42f9-9385-2935294b6de3</TermId>
-        </TermInfo>
-      </Terms>
-    </n7493b4506bf40e28c373b1e51a33445>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1355,8 +1323,65 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
+        </TermInfo>
+      </Terms>
+    </cf401361b24e474cb011be6eb76c0e76>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <k85d23755b3a46b5a51451cf336b2e9b xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k85d23755b3a46b5a51451cf336b2e9b>
+    <Topic xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Work Packages</Topic>
+    <HOMigrated xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">false</HOMigrated>
+    <ddeb1fd0a9ad4436a96525d34737dc44 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Defra Group</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0867f7b3-e76e-40ca-bb1f-5ba341a49230</TermId>
+        </TermInfo>
+      </Terms>
+    </ddeb1fd0a9ad4436a96525d34737dc44>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
+        </TermInfo>
+      </Terms>
+    </lae2bfa7b6474897ab4a53f76ea236c7>
+    <TaxCatchAll xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Value>10</Value>
+      <Value>9</Value>
+      <Value>8</Value>
+      <Value>7</Value>
+      <Value>6</Value>
+    </TaxCatchAll>
+    <fe59e9859d6a491389c5b03567f5dda5 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DDTS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4b496496-8422-4e09-ae59-802e7f67f771</TermId>
+        </TermInfo>
+      </Terms>
+    </fe59e9859d6a491389c5b03567f5dda5>
+    <Team xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">Digital Robotic Automation</Team>
+    <n7493b4506bf40e28c373b1e51a33445 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Community</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">144ac7d7-0b9a-42f9-9385-2935294b6de3</TermId>
+        </TermInfo>
+      </Terms>
+    </n7493b4506bf40e28c373b1e51a33445>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1368,20 +1393,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1cc53fe-b63d-4766-a5c8-95c307055b81"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="97f96670-c786-4b18-bf2a-32c7cc01b520"/>
-    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1408,9 +1422,20 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6890D74-70F3-4A90-9D5B-EBE10390DAD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{027021F3-0F57-4E32-99BF-C0FBFED6175E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="a1cc53fe-b63d-4766-a5c8-95c307055b81"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="97f96670-c786-4b18-bf2a-32c7cc01b520"/>
+    <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>